<commit_message>
feat: contamination, metals, change unit and norm values + graph difference from the norm + general evaluation
</commit_message>
<xml_diff>
--- a/inst/results/data_contam/metals/conversion_factors_metal.xlsx
+++ b/inst/results/data_contam/metals/conversion_factors_metal.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -387,172 +387,96 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Mercury</t>
+          <t>Cadmium</t>
         </is>
       </c>
       <c r="B2">
-        <v>0.1395</v>
+        <v>1.124</v>
       </c>
       <c r="C2">
-        <v>0.22</v>
+        <v>1.5665</v>
       </c>
       <c r="D2">
-        <v>0.6340909090909091</v>
+        <v>0.7175231407596554</v>
       </c>
       <c r="E2">
-        <v>1.577060931899641</v>
+        <v>1.393683274021352</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Cadmium</t>
+          <t>Cuivre</t>
         </is>
       </c>
       <c r="B3">
-        <v>1.124</v>
+        <v>9.407499999999999</v>
       </c>
       <c r="C3">
-        <v>1.5665</v>
+        <v>260.242</v>
       </c>
       <c r="D3">
-        <v>0.7175231407596554</v>
+        <v>0.03614904588805803</v>
       </c>
       <c r="E3">
-        <v>1.393683274021352</v>
+        <v>27.6632474089822</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Mercure</t>
         </is>
       </c>
       <c r="B4">
-        <v>1.24325</v>
+        <v>0.1395</v>
       </c>
       <c r="C4">
-        <v>1.384</v>
+        <v>0.22</v>
       </c>
       <c r="D4">
-        <v>0.8983020231213873</v>
+        <v>0.6340909090909091</v>
       </c>
       <c r="E4">
-        <v>1.11321134124271</v>
+        <v>1.577060931899641</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Zinc</t>
+          <t>Plomb</t>
         </is>
       </c>
       <c r="B5">
-        <v>144.0575</v>
+        <v>1.24325</v>
       </c>
       <c r="C5">
-        <v>2880</v>
+        <v>1.384</v>
       </c>
       <c r="D5">
-        <v>0.05001996527777778</v>
+        <v>0.8983020231213873</v>
       </c>
       <c r="E5">
-        <v>19.99201707651459</v>
+        <v>1.11321134124271</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Copper</t>
+          <t>Zinc</t>
         </is>
       </c>
       <c r="B6">
-        <v>9.407499999999999</v>
+        <v>144.0575</v>
       </c>
       <c r="C6">
-        <v>260.242</v>
+        <v>2880</v>
       </c>
       <c r="D6">
-        <v>0.03614904588805803</v>
+        <v>0.05001996527777778</v>
       </c>
       <c r="E6">
-        <v>27.6632474089822</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Nickel</t>
-        </is>
-      </c>
-      <c r="B7">
-        <v>3.4</v>
-      </c>
-      <c r="C7">
-        <v>1.38</v>
-      </c>
-      <c r="D7">
-        <v>2.463768115942029</v>
-      </c>
-      <c r="E7">
-        <v>0.4058823529411765</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Vanadium</t>
-        </is>
-      </c>
-      <c r="B8">
-        <v>2.331</v>
-      </c>
-      <c r="C8">
-        <v>1.365</v>
-      </c>
-      <c r="D8">
-        <v>1.707692307692308</v>
-      </c>
-      <c r="E8">
-        <v>0.5855855855855856</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Silver</t>
-        </is>
-      </c>
-      <c r="B9">
-        <v>0.052</v>
-      </c>
-      <c r="C9">
-        <v>10.471</v>
-      </c>
-      <c r="D9">
-        <v>0.004966096838888358</v>
-      </c>
-      <c r="E9">
-        <v>201.3653846153846</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Chromium</t>
-        </is>
-      </c>
-      <c r="B10">
-        <v>1.9845</v>
-      </c>
-      <c r="C10">
-        <v>2.1</v>
-      </c>
-      <c r="D10">
-        <v>0.9450000000000001</v>
-      </c>
-      <c r="E10">
-        <v>1.058201058201058</v>
+        <v>19.99201707651459</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: contamination, metals, delete Zinc + add general levels xslx
</commit_message>
<xml_diff>
--- a/inst/results/data_contam/metals/conversion_factors_metal.xlsx
+++ b/inst/results/data_contam/metals/conversion_factors_metal.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -460,25 +460,6 @@
         <v>1.11321134124271</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Zinc</t>
-        </is>
-      </c>
-      <c r="B6">
-        <v>144.0575</v>
-      </c>
-      <c r="C6">
-        <v>2880</v>
-      </c>
-      <c r="D6">
-        <v>0.05001996527777778</v>
-      </c>
-      <c r="E6">
-        <v>19.99201707651459</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: contamination, metal, name translation
</commit_message>
<xml_diff>
--- a/inst/results/data_contam/metals/conversion_factors_metal.xlsx
+++ b/inst/results/data_contam/metals/conversion_factors_metal.xlsx
@@ -406,7 +406,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Cuivre</t>
+          <t>Copper</t>
         </is>
       </c>
       <c r="B3">
@@ -425,39 +425,39 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Mercure</t>
+          <t>Lead</t>
         </is>
       </c>
       <c r="B4">
-        <v>0.1395</v>
+        <v>1.24325</v>
       </c>
       <c r="C4">
-        <v>0.22</v>
+        <v>1.384</v>
       </c>
       <c r="D4">
-        <v>0.6340909090909091</v>
+        <v>0.8983020231213873</v>
       </c>
       <c r="E4">
-        <v>1.577060931899641</v>
+        <v>1.11321134124271</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Plomb</t>
+          <t>Mercury</t>
         </is>
       </c>
       <c r="B5">
-        <v>1.24325</v>
+        <v>0.1395</v>
       </c>
       <c r="C5">
-        <v>1.384</v>
+        <v>0.22</v>
       </c>
       <c r="D5">
-        <v>0.8983020231213873</v>
+        <v>0.6340909090909091</v>
       </c>
       <c r="E5">
-        <v>1.11321134124271</v>
+        <v>1.577060931899641</v>
       </c>
     </row>
   </sheetData>

</xml_diff>